<commit_message>
Move generation mostly complete, missing EP and promotion still. Doesn't pass Perft testing beyond 3 with the starting position.
</commit_message>
<xml_diff>
--- a/chess-app/helper.xlsx
+++ b/chess-app/helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source_code\chess\chess-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034FDFA4-9CBA-4AC4-9191-C2F473DD3BA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024801A8-9CF3-489B-A273-375ABF69AB2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{2870E1B8-7A7D-4499-BE55-351777F5AB15}"/>
+    <workbookView xWindow="-34245" yWindow="2220" windowWidth="15420" windowHeight="15885" xr2:uid="{2870E1B8-7A7D-4499-BE55-351777F5AB15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>a8</t>
   </si>
@@ -232,13 +232,37 @@
   </si>
   <si>
     <t>Calc Rank</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +270,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +316,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -305,6 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,17 +658,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36428B0-256B-49A9-96B8-122167B6543C}">
-  <dimension ref="C7:X87"/>
+  <dimension ref="C6:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7">
         <f t="shared" ref="C7:C8" si="0">C8-8</f>
@@ -663,6 +729,9 @@
         <f t="shared" ref="J7:J8" si="7">J8-8</f>
         <v>-20</v>
       </c>
+      <c r="K7" s="7">
+        <v>8</v>
+      </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
@@ -721,6 +790,9 @@
         <f t="shared" si="7"/>
         <v>-12</v>
       </c>
+      <c r="K8" s="7">
+        <v>7</v>
+      </c>
       <c r="L8" s="4">
         <f>L7+8</f>
         <v>8</v>
@@ -787,6 +859,9 @@
         <f>J10-8</f>
         <v>-4</v>
       </c>
+      <c r="K9" s="7">
+        <v>6</v>
+      </c>
       <c r="L9">
         <f t="shared" ref="L9:L14" si="10">L8+8</f>
         <v>16</v>
@@ -845,6 +920,9 @@
       <c r="J10">
         <v>4</v>
       </c>
+      <c r="K10" s="7">
+        <v>5</v>
+      </c>
       <c r="L10">
         <f t="shared" si="10"/>
         <v>24</v>
@@ -880,7 +958,7 @@
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C11">
-        <f t="shared" ref="C9:C20" si="18">C10+8</f>
+        <f t="shared" ref="C11:C14" si="18">C10+8</f>
         <v>5</v>
       </c>
       <c r="D11" s="2">
@@ -910,6 +988,9 @@
       <c r="J11">
         <f>J10+8</f>
         <v>12</v>
+      </c>
+      <c r="K11" s="7">
+        <v>4</v>
       </c>
       <c r="L11">
         <f t="shared" si="10"/>
@@ -977,6 +1058,9 @@
         <f t="shared" ref="J12:J14" si="26">J11+8</f>
         <v>20</v>
       </c>
+      <c r="K12" s="7">
+        <v>3</v>
+      </c>
       <c r="L12">
         <f t="shared" si="10"/>
         <v>40</v>
@@ -1043,6 +1127,9 @@
         <f t="shared" si="26"/>
         <v>28</v>
       </c>
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
       <c r="L13">
         <f t="shared" si="10"/>
         <v>48</v>
@@ -1108,6 +1195,9 @@
       <c r="J14">
         <f t="shared" si="26"/>
         <v>36</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="10"/>
@@ -4382,5 +4472,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Promotion implemented. Bug fixes around the attack map. Pins are now evaluated with rays. Working through Perft debugging but passes to depth 4 on the starting board.
</commit_message>
<xml_diff>
--- a/chess-app/helper.xlsx
+++ b/chess-app/helper.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source_code\chess\chess-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024801A8-9CF3-489B-A273-375ABF69AB2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45422258-8C98-4530-8CA9-04936C9CF2E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34245" yWindow="2220" windowWidth="15420" windowHeight="15885" xr2:uid="{2870E1B8-7A7D-4499-BE55-351777F5AB15}"/>
+    <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{2870E1B8-7A7D-4499-BE55-351777F5AB15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>a8</t>
   </si>
@@ -256,6 +257,66 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>a2a3: 8457</t>
+  </si>
+  <si>
+    <t>b2b3: 9345</t>
+  </si>
+  <si>
+    <t>c2c3: 9272</t>
+  </si>
+  <si>
+    <t>d2d3: 11959</t>
+  </si>
+  <si>
+    <t>e2e3: 13134</t>
+  </si>
+  <si>
+    <t>f2f3: 8457</t>
+  </si>
+  <si>
+    <t>g2g3: 9345</t>
+  </si>
+  <si>
+    <t>h2h3: 8457</t>
+  </si>
+  <si>
+    <t>a2a4: 9329</t>
+  </si>
+  <si>
+    <t>b2b4: 9332</t>
+  </si>
+  <si>
+    <t>c2c4: 9744</t>
+  </si>
+  <si>
+    <t>d2d4: 12435</t>
+  </si>
+  <si>
+    <t>e2e4: 13160</t>
+  </si>
+  <si>
+    <t>f2f4: 8929</t>
+  </si>
+  <si>
+    <t>g2g4: 9328</t>
+  </si>
+  <si>
+    <t>h2h4: 9329</t>
+  </si>
+  <si>
+    <t>b1a3: 8885</t>
+  </si>
+  <si>
+    <t>b1c3: 9755</t>
+  </si>
+  <si>
+    <t>g1f3: 9748</t>
+  </si>
+  <si>
+    <t>g1h3: 8881</t>
   </si>
 </sst>
 </file>
@@ -660,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36428B0-256B-49A9-96B8-122167B6543C}">
   <dimension ref="C6:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -4474,4 +4535,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3890B13-C358-456C-98AE-7F6A57C46179}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More perft fixes, including EP into check moves and preventing the king from moving into check from a pinned piece.
</commit_message>
<xml_diff>
--- a/chess-app/helper.xlsx
+++ b/chess-app/helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source_code\chess\chess-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45422258-8C98-4530-8CA9-04936C9CF2E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22CB26F-DFAA-446D-9136-B38DBCFFA0AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37590" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{2870E1B8-7A7D-4499-BE55-351777F5AB15}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>a8</t>
   </si>
@@ -259,64 +259,205 @@
     <t>h</t>
   </si>
   <si>
-    <t>a2a3: 8457</t>
-  </si>
-  <si>
-    <t>b2b3: 9345</t>
-  </si>
-  <si>
-    <t>c2c3: 9272</t>
-  </si>
-  <si>
-    <t>d2d3: 11959</t>
-  </si>
-  <si>
-    <t>e2e3: 13134</t>
-  </si>
-  <si>
-    <t>f2f3: 8457</t>
-  </si>
-  <si>
-    <t>g2g3: 9345</t>
-  </si>
-  <si>
-    <t>h2h3: 8457</t>
-  </si>
-  <si>
-    <t>a2a4: 9329</t>
-  </si>
-  <si>
-    <t>b2b4: 9332</t>
-  </si>
-  <si>
-    <t>c2c4: 9744</t>
-  </si>
-  <si>
-    <t>d2d4: 12435</t>
-  </si>
-  <si>
-    <t>e2e4: 13160</t>
-  </si>
-  <si>
-    <t>f2f4: 8929</t>
-  </si>
-  <si>
-    <t>g2g4: 9328</t>
-  </si>
-  <si>
-    <t>h2h4: 9329</t>
-  </si>
-  <si>
-    <t>b1a3: 8885</t>
-  </si>
-  <si>
-    <t>b1c3: 9755</t>
-  </si>
-  <si>
-    <t>g1f3: 9748</t>
-  </si>
-  <si>
-    <t>g1h3: 8881</t>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>a2a3: 34</t>
+  </si>
+  <si>
+    <t>a2a4: 34</t>
+  </si>
+  <si>
+    <t>b1a3: 34</t>
+  </si>
+  <si>
+    <t>b1c3: 34</t>
+  </si>
+  <si>
+    <t>b1d2: 34</t>
+  </si>
+  <si>
+    <t>b2b3: 34</t>
+  </si>
+  <si>
+    <t>b2b4: 33</t>
+  </si>
+  <si>
+    <t>c1d2: 34</t>
+  </si>
+  <si>
+    <t>c1e3: 34</t>
+  </si>
+  <si>
+    <t>c1f4: 34</t>
+  </si>
+  <si>
+    <t>c1g5: 32</t>
+  </si>
+  <si>
+    <t>c1h6: 30</t>
+  </si>
+  <si>
+    <t>c2c3: 34</t>
+  </si>
+  <si>
+    <t>c4a6: 33</t>
+  </si>
+  <si>
+    <t>c4b3: 34</t>
+  </si>
+  <si>
+    <t>c4b5: 34</t>
+  </si>
+  <si>
+    <t>c4d3: 34</t>
+  </si>
+  <si>
+    <t>c4d5: 35</t>
+  </si>
+  <si>
+    <t>c4e6: 35</t>
+  </si>
+  <si>
+    <t>c4f7: 32</t>
+  </si>
+  <si>
+    <t>d1d2: 34</t>
+  </si>
+  <si>
+    <t>d1d3: 34</t>
+  </si>
+  <si>
+    <t>d1d4: 34</t>
+  </si>
+  <si>
+    <t>d1d5: 35</t>
+  </si>
+  <si>
+    <t>d1d6: 27</t>
+  </si>
+  <si>
+    <t>d7c8b: 46</t>
+  </si>
+  <si>
+    <t>d7c8n: 46</t>
+  </si>
+  <si>
+    <t>d7c8q: 46</t>
+  </si>
+  <si>
+    <t>d7c8r: 46</t>
+  </si>
+  <si>
+    <t>e1d2: 36</t>
+  </si>
+  <si>
+    <t>e1f1: 35</t>
+  </si>
+  <si>
+    <t>e1f2: 29</t>
+  </si>
+  <si>
+    <t>e2c3: 35</t>
+  </si>
+  <si>
+    <t>e2d4: 35</t>
+  </si>
+  <si>
+    <t>e2f4: 35</t>
+  </si>
+  <si>
+    <t>e2g1: 35</t>
+  </si>
+  <si>
+    <t>e2g3: 35</t>
+  </si>
+  <si>
+    <t>g2g3: 35</t>
+  </si>
+  <si>
+    <t>g2g4: 35</t>
+  </si>
+  <si>
+    <t>h1f1: 35</t>
+  </si>
+  <si>
+    <t>h1g1: 35</t>
+  </si>
+  <si>
+    <t>h2h3: 35</t>
+  </si>
+  <si>
+    <t>h2h4: 35</t>
+  </si>
+  <si>
+    <t>g2g3: 34</t>
+  </si>
+  <si>
+    <t>h2h3: 34</t>
+  </si>
+  <si>
+    <t>g2g4: 34</t>
+  </si>
+  <si>
+    <t>h2h4: 34</t>
+  </si>
+  <si>
+    <t>d7c8q: 31</t>
+  </si>
+  <si>
+    <t>d7c8r: 31</t>
+  </si>
+  <si>
+    <t>d7c8b: 41</t>
+  </si>
+  <si>
+    <t>d7c8n: 41</t>
+  </si>
+  <si>
+    <t>e2g1: 34</t>
+  </si>
+  <si>
+    <t>e2c3: 34</t>
+  </si>
+  <si>
+    <t>e2g3: 34</t>
+  </si>
+  <si>
+    <t>e2d4: 34</t>
+  </si>
+  <si>
+    <t>e2f4: 34</t>
+  </si>
+  <si>
+    <t>c1h6: 31</t>
+  </si>
+  <si>
+    <t>h1f1: 34</t>
+  </si>
+  <si>
+    <t>h1g1: 34</t>
+  </si>
+  <si>
+    <t>d1d6: 28</t>
+  </si>
+  <si>
+    <t>e1f1: 34</t>
+  </si>
+  <si>
+    <t>e1d2: 34</t>
+  </si>
+  <si>
+    <t>e1f2: 28</t>
+  </si>
+  <si>
+    <t>e1g1: 34</t>
+  </si>
+  <si>
+    <t>FEN rnbq1k1r/pp1Pbppp/2p5/8/2B5/8/PPP1NnPP/RNBQK2R w KQ - 1 8 Depth 2</t>
   </si>
 </sst>
 </file>
@@ -340,7 +481,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +524,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -396,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -405,6 +558,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36428B0-256B-49A9-96B8-122167B6543C}">
-  <dimension ref="C6:X87"/>
+  <dimension ref="C6:AE87"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +887,7 @@
     <col min="11" max="11" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
       <c r="K6" s="7"/>
       <c r="L6" s="7" t="s">
         <v>66</v>
@@ -757,7 +914,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C7">
         <f t="shared" ref="C7:C8" si="0">C8-8</f>
         <v>-27</v>
@@ -793,19 +950,19 @@
       <c r="K7" s="7">
         <v>8</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="3">
         <v>2</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>3</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>4</v>
       </c>
       <c r="Q7">
@@ -818,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C8">
         <f t="shared" si="0"/>
         <v>-19</v>
@@ -854,15 +1011,15 @@
       <c r="K8" s="7">
         <v>7</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <f>L7+8</f>
         <v>8</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <f t="shared" ref="M8:S8" si="8">M7+8</f>
         <v>9</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="3">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
@@ -887,7 +1044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C9">
         <f t="shared" ref="C9:I9" si="9">C10-8</f>
         <v>-11</v>
@@ -923,23 +1080,23 @@
       <c r="K9" s="7">
         <v>6</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <f t="shared" ref="L9:L14" si="10">L8+8</f>
         <v>16</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <f t="shared" ref="M9:M14" si="11">M8+8</f>
         <v>17</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="3">
         <f t="shared" ref="N9:N14" si="12">N8+8</f>
         <v>18</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="3">
         <f t="shared" ref="O9:O14" si="13">O8+8</f>
         <v>19</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="3">
         <f t="shared" ref="P9:P14" si="14">P8+8</f>
         <v>20</v>
       </c>
@@ -955,8 +1112,18 @@
         <f t="shared" ref="S9:S14" si="17">S8+8</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <v>4</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" ref="AD9:AD12" si="18">2*(2^AE9)</f>
+        <v>4</v>
+      </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>-3</v>
       </c>
@@ -984,7 +1151,7 @@
       <c r="K10" s="7">
         <v>5</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
@@ -992,7 +1159,7 @@
         <f t="shared" si="11"/>
         <v>25</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <f t="shared" si="12"/>
         <v>26</v>
       </c>
@@ -1000,7 +1167,7 @@
         <f>O9+8</f>
         <v>27</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="3">
         <f t="shared" si="14"/>
         <v>28</v>
       </c>
@@ -1016,34 +1183,44 @@
         <f t="shared" si="17"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>8</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="AE10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C11">
-        <f t="shared" ref="C11:C14" si="18">C10+8</f>
+        <f t="shared" ref="C11:C14" si="19">C10+8</f>
         <v>5</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:I11" si="19">D10+8</f>
+        <f t="shared" ref="D11:I11" si="20">D10+8</f>
         <v>6</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="I11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>11</v>
       </c>
       <c r="J11">
@@ -1053,7 +1230,7 @@
       <c r="K11" s="7">
         <v>4</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <f t="shared" si="10"/>
         <v>32</v>
       </c>
@@ -1061,15 +1238,15 @@
         <f t="shared" si="11"/>
         <v>33</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="9">
         <f t="shared" si="12"/>
         <v>34</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="3">
         <f t="shared" si="13"/>
         <v>35</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="3">
         <f t="shared" si="14"/>
         <v>36</v>
       </c>
@@ -1085,44 +1262,54 @@
         <f t="shared" si="17"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="AC11">
+        <v>16</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>13</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D14" si="20">D11+8</f>
+        <f t="shared" ref="D12:D14" si="21">D11+8</f>
         <v>14</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" ref="E12:E14" si="21">E11+8</f>
+        <f t="shared" ref="E12:E14" si="22">E11+8</f>
         <v>15</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F14" si="22">F11+8</f>
+        <f t="shared" ref="F12:F14" si="23">F11+8</f>
         <v>16</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G14" si="23">G11+8</f>
+        <f t="shared" ref="G12:G14" si="24">G11+8</f>
         <v>17</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H14" si="24">H11+8</f>
+        <f t="shared" ref="H12:H14" si="25">H11+8</f>
         <v>18</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I14" si="25">I11+8</f>
+        <f t="shared" ref="I12:I14" si="26">I11+8</f>
         <v>19</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J14" si="26">J11+8</f>
+        <f t="shared" ref="J12:J14" si="27">J11+8</f>
         <v>20</v>
       </c>
       <c r="K12" s="7">
         <v>3</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
@@ -1134,7 +1321,7 @@
         <f t="shared" si="12"/>
         <v>42</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="8">
         <f t="shared" si="13"/>
         <v>43</v>
       </c>
@@ -1154,38 +1341,48 @@
         <f t="shared" si="17"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>32</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="18"/>
+        <v>32</v>
+      </c>
+      <c r="AE12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C13">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>21</v>
       </c>
       <c r="D13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>22</v>
       </c>
       <c r="E13">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>23</v>
       </c>
       <c r="F13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>24</v>
       </c>
       <c r="G13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>25</v>
       </c>
       <c r="H13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>26</v>
       </c>
       <c r="I13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>27</v>
       </c>
       <c r="J13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>28</v>
       </c>
       <c r="K13" s="7">
@@ -1224,37 +1421,37 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>29</v>
       </c>
       <c r="D14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="E14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>31</v>
       </c>
       <c r="F14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>32</v>
       </c>
       <c r="G14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>33</v>
       </c>
       <c r="H14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>34</v>
       </c>
       <c r="I14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>35</v>
       </c>
       <c r="J14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>36</v>
       </c>
       <c r="K14" s="7">
@@ -1313,8 +1510,14 @@
         <v>1</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" ref="E18:E80" si="27">_xlfn.CONCAT(D18,"=",C18,",")</f>
+        <f t="shared" ref="E18:E80" si="28">_xlfn.CONCAT(D18,"=",C18,",")</f>
         <v>b8=1,</v>
+      </c>
+      <c r="M18" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="3:24" x14ac:dyDescent="0.25">
@@ -1325,8 +1528,14 @@
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c8=2,</v>
+      </c>
+      <c r="M19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19">
+        <v>-6</v>
       </c>
     </row>
     <row r="20" spans="3:24" x14ac:dyDescent="0.25">
@@ -1337,7 +1546,7 @@
         <v>3</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d8=3,</v>
       </c>
     </row>
@@ -1349,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e8=4,</v>
       </c>
     </row>
@@ -1361,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f8=5,</v>
       </c>
     </row>
@@ -1373,7 +1582,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g8=6,</v>
       </c>
     </row>
@@ -1385,7 +1594,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h8=7,</v>
       </c>
       <c r="K24" s="6">
@@ -1439,7 +1648,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a7=8,</v>
       </c>
       <c r="K25" s="6">
@@ -1447,55 +1656,55 @@
         <v>14</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" ref="L25:X25" si="28">L24+14</f>
+        <f t="shared" ref="L25:X25" si="29">L24+14</f>
         <v>15</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>16</v>
       </c>
       <c r="N25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>17</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>18</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>19</v>
       </c>
       <c r="Q25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>20</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>21</v>
       </c>
       <c r="S25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>22</v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="U25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>24</v>
       </c>
       <c r="V25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>25</v>
       </c>
       <c r="W25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>26</v>
       </c>
       <c r="X25" s="6">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>27</v>
       </c>
     </row>
@@ -1507,65 +1716,65 @@
         <v>9</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b7=9,</v>
       </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="6">
-        <f t="shared" ref="K26:K38" si="29">K25+14</f>
+        <f t="shared" ref="K26:K38" si="30">K25+14</f>
         <v>28</v>
       </c>
       <c r="L26" s="6">
-        <f t="shared" ref="L26:L38" si="30">L25+14</f>
+        <f t="shared" ref="L26:L38" si="31">L25+14</f>
         <v>29</v>
       </c>
       <c r="M26" s="6">
-        <f t="shared" ref="M26:M38" si="31">M25+14</f>
+        <f t="shared" ref="M26:M38" si="32">M25+14</f>
         <v>30</v>
       </c>
       <c r="N26" s="6">
-        <f t="shared" ref="N26:N38" si="32">N25+14</f>
+        <f t="shared" ref="N26:N38" si="33">N25+14</f>
         <v>31</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" ref="O26:O38" si="33">O25+14</f>
+        <f t="shared" ref="O26:O38" si="34">O25+14</f>
         <v>32</v>
       </c>
       <c r="P26" s="6">
-        <f t="shared" ref="P26:P38" si="34">P25+14</f>
+        <f t="shared" ref="P26:P38" si="35">P25+14</f>
         <v>33</v>
       </c>
       <c r="Q26" s="6">
-        <f t="shared" ref="Q26:Q38" si="35">Q25+14</f>
+        <f t="shared" ref="Q26:Q38" si="36">Q25+14</f>
         <v>34</v>
       </c>
       <c r="R26" s="6">
-        <f t="shared" ref="R26:R38" si="36">R25+14</f>
+        <f t="shared" ref="R26:R38" si="37">R25+14</f>
         <v>35</v>
       </c>
       <c r="S26" s="6">
-        <f t="shared" ref="S26:S38" si="37">S25+14</f>
+        <f t="shared" ref="S26:S38" si="38">S25+14</f>
         <v>36</v>
       </c>
       <c r="T26" s="6">
-        <f t="shared" ref="T26:T38" si="38">T25+14</f>
+        <f t="shared" ref="T26:T38" si="39">T25+14</f>
         <v>37</v>
       </c>
       <c r="U26" s="6">
-        <f t="shared" ref="U26:U38" si="39">U25+14</f>
+        <f t="shared" ref="U26:U38" si="40">U25+14</f>
         <v>38</v>
       </c>
       <c r="V26" s="6">
-        <f t="shared" ref="V26:V38" si="40">V25+14</f>
+        <f t="shared" ref="V26:V38" si="41">V25+14</f>
         <v>39</v>
       </c>
       <c r="W26" s="6">
-        <f t="shared" ref="W26:W38" si="41">W25+14</f>
+        <f t="shared" ref="W26:W38" si="42">W25+14</f>
         <v>40</v>
       </c>
       <c r="X26" s="6">
-        <f t="shared" ref="X26:X38" si="42">X25+14</f>
+        <f t="shared" ref="X26:X38" si="43">X25+14</f>
         <v>41</v>
       </c>
     </row>
@@ -1577,65 +1786,65 @@
         <v>10</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c7=10,</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>42</v>
       </c>
       <c r="L27" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>43</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>44</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>45</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>46</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>47</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>48</v>
       </c>
       <c r="R27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>49</v>
       </c>
       <c r="S27" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>50</v>
       </c>
       <c r="T27" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>51</v>
       </c>
       <c r="U27" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>52</v>
       </c>
       <c r="V27" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>53</v>
       </c>
       <c r="W27" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>54</v>
       </c>
       <c r="X27" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>55</v>
       </c>
     </row>
@@ -1647,65 +1856,65 @@
         <v>11</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d7=11,</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>56</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>57</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>59</v>
       </c>
       <c r="O28" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>60</v>
       </c>
       <c r="P28" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>61</v>
       </c>
       <c r="Q28" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>62</v>
       </c>
       <c r="R28" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>63</v>
       </c>
       <c r="S28" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>64</v>
       </c>
       <c r="T28" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>65</v>
       </c>
       <c r="U28" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>66</v>
       </c>
       <c r="V28" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>67</v>
       </c>
       <c r="W28" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
       <c r="X28" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>69</v>
       </c>
     </row>
@@ -1717,65 +1926,65 @@
         <v>12</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e7=12,</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>70</v>
       </c>
       <c r="L29" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>71</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>72</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>73</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>74</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>75</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>76</v>
       </c>
       <c r="R29" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>77</v>
       </c>
       <c r="S29" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>78</v>
       </c>
       <c r="T29" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>79</v>
       </c>
       <c r="U29" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>80</v>
       </c>
       <c r="V29" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>81</v>
       </c>
       <c r="W29" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>82</v>
       </c>
       <c r="X29" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>83</v>
       </c>
     </row>
@@ -1787,65 +1996,65 @@
         <v>13</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f7=13,</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>84</v>
       </c>
       <c r="L30" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>85</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>86</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>87</v>
       </c>
       <c r="O30" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>88</v>
       </c>
       <c r="P30" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>89</v>
       </c>
       <c r="Q30" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>90</v>
       </c>
       <c r="R30" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>91</v>
       </c>
       <c r="S30" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>92</v>
       </c>
       <c r="T30" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>93</v>
       </c>
       <c r="U30" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>94</v>
       </c>
       <c r="V30" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>95</v>
       </c>
       <c r="W30" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>96</v>
       </c>
       <c r="X30" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>97</v>
       </c>
     </row>
@@ -1857,65 +2066,65 @@
         <v>14</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g7=14,</v>
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>98</v>
       </c>
       <c r="L31" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>99</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>100</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>101</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>102</v>
       </c>
       <c r="P31" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>103</v>
       </c>
       <c r="Q31" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>104</v>
       </c>
       <c r="R31" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>105</v>
       </c>
       <c r="S31" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>106</v>
       </c>
       <c r="T31" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>107</v>
       </c>
       <c r="U31" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>108</v>
       </c>
       <c r="V31" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>109</v>
       </c>
       <c r="W31" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>110</v>
       </c>
       <c r="X31" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>111</v>
       </c>
     </row>
@@ -1927,65 +2136,65 @@
         <v>15</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h7=15,</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>112</v>
       </c>
       <c r="L32" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>113</v>
       </c>
       <c r="M32" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>114</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>115</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>116</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>117</v>
       </c>
       <c r="Q32" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>118</v>
       </c>
       <c r="R32" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>119</v>
       </c>
       <c r="S32" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>120</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>121</v>
       </c>
       <c r="U32" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>122</v>
       </c>
       <c r="V32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>123</v>
       </c>
       <c r="W32" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>124</v>
       </c>
       <c r="X32" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>125</v>
       </c>
     </row>
@@ -1997,65 +2206,65 @@
         <v>16</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a6=16,</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>126</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>127</v>
       </c>
       <c r="M33" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>128</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>129</v>
       </c>
       <c r="O33" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>130</v>
       </c>
       <c r="P33" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>131</v>
       </c>
       <c r="Q33" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>132</v>
       </c>
       <c r="R33" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>133</v>
       </c>
       <c r="S33" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>134</v>
       </c>
       <c r="T33" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>135</v>
       </c>
       <c r="U33" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>136</v>
       </c>
       <c r="V33" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>137</v>
       </c>
       <c r="W33" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>138</v>
       </c>
       <c r="X33" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>139</v>
       </c>
     </row>
@@ -2067,65 +2276,65 @@
         <v>17</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b6=17,</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>140</v>
       </c>
       <c r="L34" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>141</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>142</v>
       </c>
       <c r="N34" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>143</v>
       </c>
       <c r="O34" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>144</v>
       </c>
       <c r="P34" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>145</v>
       </c>
       <c r="Q34" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>146</v>
       </c>
       <c r="R34" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>147</v>
       </c>
       <c r="S34" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>148</v>
       </c>
       <c r="T34" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>149</v>
       </c>
       <c r="U34" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>150</v>
       </c>
       <c r="V34" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>151</v>
       </c>
       <c r="W34" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>152</v>
       </c>
       <c r="X34" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>153</v>
       </c>
     </row>
@@ -2137,65 +2346,65 @@
         <v>18</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c6=18,</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>154</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>155</v>
       </c>
       <c r="M35" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>156</v>
       </c>
       <c r="N35" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>157</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>158</v>
       </c>
       <c r="P35" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>159</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>160</v>
       </c>
       <c r="R35" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>161</v>
       </c>
       <c r="S35" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>162</v>
       </c>
       <c r="T35" s="6">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>163</v>
       </c>
       <c r="U35" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>164</v>
       </c>
       <c r="V35" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>165</v>
       </c>
       <c r="W35" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>166</v>
       </c>
       <c r="X35" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>167</v>
       </c>
     </row>
@@ -2207,65 +2416,65 @@
         <v>19</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d6=19,</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>168</v>
       </c>
       <c r="L36" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>169</v>
       </c>
       <c r="M36" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>170</v>
       </c>
       <c r="N36" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>171</v>
       </c>
       <c r="O36" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>172</v>
       </c>
       <c r="P36" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>173</v>
       </c>
       <c r="Q36" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>174</v>
       </c>
       <c r="R36" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>175</v>
       </c>
       <c r="S36" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>176</v>
       </c>
       <c r="T36" s="6">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>177</v>
       </c>
       <c r="U36" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>178</v>
       </c>
       <c r="V36" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>179</v>
       </c>
       <c r="W36" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>180</v>
       </c>
       <c r="X36" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>181</v>
       </c>
     </row>
@@ -2277,65 +2486,65 @@
         <v>20</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e6=20,</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>182</v>
       </c>
       <c r="L37" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>183</v>
       </c>
       <c r="M37" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>184</v>
       </c>
       <c r="N37" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>185</v>
       </c>
       <c r="O37" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>186</v>
       </c>
       <c r="P37" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>187</v>
       </c>
       <c r="Q37" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>188</v>
       </c>
       <c r="R37" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>189</v>
       </c>
       <c r="S37" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>190</v>
       </c>
       <c r="T37" s="6">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>191</v>
       </c>
       <c r="U37" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>192</v>
       </c>
       <c r="V37" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>193</v>
       </c>
       <c r="W37" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>194</v>
       </c>
       <c r="X37" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>195</v>
       </c>
     </row>
@@ -2347,65 +2556,65 @@
         <v>21</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f6=21,</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>196</v>
       </c>
       <c r="L38" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>197</v>
       </c>
       <c r="M38" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>198</v>
       </c>
       <c r="N38" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>199</v>
       </c>
       <c r="O38" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>200</v>
       </c>
       <c r="P38" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>201</v>
       </c>
       <c r="Q38" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>202</v>
       </c>
       <c r="R38" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>203</v>
       </c>
       <c r="S38" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>204</v>
       </c>
       <c r="T38" s="6">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>205</v>
       </c>
       <c r="U38" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>206</v>
       </c>
       <c r="V38" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>207</v>
       </c>
       <c r="W38" s="6">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>208</v>
       </c>
       <c r="X38" s="6">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>209</v>
       </c>
     </row>
@@ -2417,7 +2626,7 @@
         <v>22</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g6=22,</v>
       </c>
       <c r="I39" s="3"/>
@@ -2439,7 +2648,7 @@
         <v>23</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h6=23,</v>
       </c>
     </row>
@@ -2451,7 +2660,7 @@
         <v>24</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a5=24,</v>
       </c>
     </row>
@@ -2463,7 +2672,7 @@
         <v>25</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b5=25,</v>
       </c>
     </row>
@@ -2475,7 +2684,7 @@
         <v>26</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c5=26,</v>
       </c>
       <c r="L43" t="s">
@@ -2493,7 +2702,7 @@
         <v>27</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d5=27,</v>
       </c>
       <c r="L44">
@@ -2508,31 +2717,31 @@
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44:U45" si="43">O27-45-6*$M44</f>
+        <f t="shared" ref="O44:U45" si="44">O27-45-6*$M44</f>
         <v>1</v>
       </c>
       <c r="P44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>3</v>
       </c>
       <c r="R44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>4</v>
       </c>
       <c r="S44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>5</v>
       </c>
       <c r="T44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>6</v>
       </c>
       <c r="U44">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
     </row>
@@ -2544,11 +2753,11 @@
         <v>28</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e5=28,</v>
       </c>
       <c r="L45">
-        <f t="shared" ref="L45:L51" si="44">_xlfn.FLOOR.MATH(N28/14)-3</f>
+        <f t="shared" ref="L45:L51" si="45">_xlfn.FLOOR.MATH(N28/14)-3</f>
         <v>1</v>
       </c>
       <c r="M45">
@@ -2559,31 +2768,31 @@
         <v>8</v>
       </c>
       <c r="O45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>9</v>
       </c>
       <c r="P45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>11</v>
       </c>
       <c r="R45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>12</v>
       </c>
       <c r="S45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>13</v>
       </c>
       <c r="T45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14</v>
       </c>
       <c r="U45">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>15</v>
       </c>
     </row>
@@ -2595,46 +2804,46 @@
         <v>29</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f5=29,</v>
       </c>
       <c r="L46">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M46">
         <v>2</v>
       </c>
       <c r="N46">
-        <f t="shared" ref="N46:U46" si="45">N29-45-6*$M46</f>
+        <f t="shared" ref="N46:U46" si="46">N29-45-6*$M46</f>
         <v>16</v>
       </c>
       <c r="O46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>17</v>
       </c>
       <c r="P46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>18</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>19</v>
       </c>
       <c r="R46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>20</v>
       </c>
       <c r="S46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>21</v>
       </c>
       <c r="T46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>22</v>
       </c>
       <c r="U46">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>23</v>
       </c>
     </row>
@@ -2646,46 +2855,46 @@
         <v>30</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g5=30,</v>
       </c>
       <c r="L47">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>3</v>
       </c>
       <c r="M47">
         <v>3</v>
       </c>
       <c r="N47">
-        <f t="shared" ref="N47:U47" si="46">N30-45-6*$M47</f>
+        <f t="shared" ref="N47:U47" si="47">N30-45-6*$M47</f>
         <v>24</v>
       </c>
       <c r="O47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>25</v>
       </c>
       <c r="P47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>26</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>27</v>
       </c>
       <c r="R47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>28</v>
       </c>
       <c r="S47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>29</v>
       </c>
       <c r="T47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>30</v>
       </c>
       <c r="U47">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>31</v>
       </c>
     </row>
@@ -2697,46 +2906,46 @@
         <v>31</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h5=31,</v>
       </c>
       <c r="L48">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="M48">
         <v>4</v>
       </c>
       <c r="N48">
-        <f t="shared" ref="N48:U48" si="47">N31-45-6*$M48</f>
+        <f t="shared" ref="N48:U48" si="48">N31-45-6*$M48</f>
         <v>32</v>
       </c>
       <c r="O48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>33</v>
       </c>
       <c r="P48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>34</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>35</v>
       </c>
       <c r="R48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>36</v>
       </c>
       <c r="S48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>37</v>
       </c>
       <c r="T48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>38</v>
       </c>
       <c r="U48">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>39</v>
       </c>
     </row>
@@ -2748,46 +2957,46 @@
         <v>32</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a4=32,</v>
       </c>
       <c r="L49">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>5</v>
       </c>
       <c r="M49">
         <v>5</v>
       </c>
       <c r="N49">
-        <f t="shared" ref="N49:U49" si="48">N32-45-6*$M49</f>
+        <f t="shared" ref="N49:U49" si="49">N32-45-6*$M49</f>
         <v>40</v>
       </c>
       <c r="O49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>41</v>
       </c>
       <c r="P49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>42</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>43</v>
       </c>
       <c r="R49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>44</v>
       </c>
       <c r="S49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>45</v>
       </c>
       <c r="T49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>46</v>
       </c>
       <c r="U49">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>47</v>
       </c>
     </row>
@@ -2799,46 +3008,46 @@
         <v>33</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b4=33,</v>
       </c>
       <c r="L50">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>6</v>
       </c>
       <c r="M50">
         <v>6</v>
       </c>
       <c r="N50">
-        <f t="shared" ref="N50:U50" si="49">N33-45-6*$M50</f>
+        <f t="shared" ref="N50:U50" si="50">N33-45-6*$M50</f>
         <v>48</v>
       </c>
       <c r="O50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>49</v>
       </c>
       <c r="P50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>50</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>51</v>
       </c>
       <c r="R50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>52</v>
       </c>
       <c r="S50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>53</v>
       </c>
       <c r="T50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>54</v>
       </c>
       <c r="U50">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>55</v>
       </c>
     </row>
@@ -2850,46 +3059,46 @@
         <v>34</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c4=34,</v>
       </c>
       <c r="L51">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>7</v>
       </c>
       <c r="M51">
         <v>7</v>
       </c>
       <c r="N51">
-        <f t="shared" ref="N51:U51" si="50">N34-45-6*$M51</f>
+        <f t="shared" ref="N51:U51" si="51">N34-45-6*$M51</f>
         <v>56</v>
       </c>
       <c r="O51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>57</v>
       </c>
       <c r="P51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>58</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>59</v>
       </c>
       <c r="R51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>60</v>
       </c>
       <c r="S51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>61</v>
       </c>
       <c r="T51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>62</v>
       </c>
       <c r="U51">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>63</v>
       </c>
     </row>
@@ -2901,7 +3110,7 @@
         <v>35</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d4=35,</v>
       </c>
     </row>
@@ -2913,7 +3122,7 @@
         <v>36</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e4=36,</v>
       </c>
     </row>
@@ -2925,7 +3134,7 @@
         <v>37</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f4=37,</v>
       </c>
     </row>
@@ -2937,63 +3146,63 @@
         <v>38</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g4=38,</v>
       </c>
       <c r="K55" s="6">
-        <f t="shared" ref="K55:K59" si="51">K56-14</f>
+        <f t="shared" ref="K55:K59" si="52">K56-14</f>
         <v>-90</v>
       </c>
       <c r="L55" s="6">
-        <f t="shared" ref="L55:L59" si="52">L56-14</f>
+        <f t="shared" ref="L55:L59" si="53">L56-14</f>
         <v>-89</v>
       </c>
       <c r="M55" s="6">
-        <f t="shared" ref="M55:M59" si="53">M56-14</f>
+        <f t="shared" ref="M55:M59" si="54">M56-14</f>
         <v>-88</v>
       </c>
       <c r="N55" s="6">
-        <f t="shared" ref="N55:N59" si="54">N56-14</f>
+        <f t="shared" ref="N55:N59" si="55">N56-14</f>
         <v>-87</v>
       </c>
       <c r="O55" s="6">
-        <f t="shared" ref="O55:O59" si="55">O56-14</f>
+        <f t="shared" ref="O55:O59" si="56">O56-14</f>
         <v>-86</v>
       </c>
       <c r="P55" s="6">
-        <f t="shared" ref="P55:P59" si="56">P56-14</f>
+        <f t="shared" ref="P55:P59" si="57">P56-14</f>
         <v>-85</v>
       </c>
       <c r="Q55" s="6">
-        <f t="shared" ref="Q55:Q59" si="57">Q56-14</f>
+        <f t="shared" ref="Q55:Q59" si="58">Q56-14</f>
         <v>-84</v>
       </c>
       <c r="R55" s="6">
-        <f t="shared" ref="R55:R59" si="58">R56-14</f>
+        <f t="shared" ref="R55:R59" si="59">R56-14</f>
         <v>-83</v>
       </c>
       <c r="S55" s="6">
-        <f t="shared" ref="S55:S59" si="59">S56-14</f>
+        <f t="shared" ref="S55:S59" si="60">S56-14</f>
         <v>-82</v>
       </c>
       <c r="T55" s="6">
-        <f t="shared" ref="T55:T59" si="60">T56-14</f>
+        <f t="shared" ref="T55:T59" si="61">T56-14</f>
         <v>-81</v>
       </c>
       <c r="U55" s="6">
-        <f t="shared" ref="U55:U59" si="61">U56-14</f>
+        <f t="shared" ref="U55:U59" si="62">U56-14</f>
         <v>-80</v>
       </c>
       <c r="V55" s="6">
-        <f t="shared" ref="V55:V59" si="62">V56-14</f>
+        <f t="shared" ref="V55:V59" si="63">V56-14</f>
         <v>-79</v>
       </c>
       <c r="W55" s="6">
-        <f t="shared" ref="W55:W59" si="63">W56-14</f>
+        <f t="shared" ref="W55:W59" si="64">W56-14</f>
         <v>-78</v>
       </c>
       <c r="X55" s="6">
-        <f t="shared" ref="X55:X59" si="64">X56-14</f>
+        <f t="shared" ref="X55:X59" si="65">X56-14</f>
         <v>-77</v>
       </c>
     </row>
@@ -3005,63 +3214,63 @@
         <v>39</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h4=39,</v>
       </c>
       <c r="K56" s="6">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-76</v>
       </c>
       <c r="L56" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-75</v>
       </c>
       <c r="M56" s="6">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-74</v>
       </c>
       <c r="N56" s="6">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>-73</v>
       </c>
       <c r="O56" s="6">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>-72</v>
       </c>
       <c r="P56" s="6">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>-71</v>
       </c>
       <c r="Q56" s="6">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>-70</v>
       </c>
       <c r="R56" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-69</v>
       </c>
       <c r="S56" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>-68</v>
       </c>
       <c r="T56" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-67</v>
       </c>
       <c r="U56" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-66</v>
       </c>
       <c r="V56" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-65</v>
       </c>
       <c r="W56" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>-64</v>
       </c>
       <c r="X56" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>-63</v>
       </c>
     </row>
@@ -3073,63 +3282,63 @@
         <v>40</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a3=40,</v>
       </c>
       <c r="K57" s="6">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-62</v>
       </c>
       <c r="L57" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-61</v>
       </c>
       <c r="M57" s="6">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-60</v>
       </c>
       <c r="N57" s="6">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>-59</v>
       </c>
       <c r="O57" s="6">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>-58</v>
       </c>
       <c r="P57" s="6">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>-57</v>
       </c>
       <c r="Q57" s="6">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>-56</v>
       </c>
       <c r="R57" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-55</v>
       </c>
       <c r="S57" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>-54</v>
       </c>
       <c r="T57" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-53</v>
       </c>
       <c r="U57" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-52</v>
       </c>
       <c r="V57" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-51</v>
       </c>
       <c r="W57" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>-50</v>
       </c>
       <c r="X57" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>-49</v>
       </c>
     </row>
@@ -3141,63 +3350,63 @@
         <v>41</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b3=41,</v>
       </c>
       <c r="K58" s="6">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-48</v>
       </c>
       <c r="L58" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-47</v>
       </c>
       <c r="M58" s="6">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-46</v>
       </c>
       <c r="N58" s="6">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>-45</v>
       </c>
       <c r="O58" s="6">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>-44</v>
       </c>
       <c r="P58" s="6">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>-43</v>
       </c>
       <c r="Q58" s="6">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>-42</v>
       </c>
       <c r="R58" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-41</v>
       </c>
       <c r="S58" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>-40</v>
       </c>
       <c r="T58" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-39</v>
       </c>
       <c r="U58" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-38</v>
       </c>
       <c r="V58" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-37</v>
       </c>
       <c r="W58" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>-36</v>
       </c>
       <c r="X58" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>-35</v>
       </c>
     </row>
@@ -3209,63 +3418,63 @@
         <v>42</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c3=42,</v>
       </c>
       <c r="K59" s="6">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-34</v>
       </c>
       <c r="L59" s="6">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-33</v>
       </c>
       <c r="M59" s="6">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-32</v>
       </c>
       <c r="N59" s="6">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>-31</v>
       </c>
       <c r="O59" s="6">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>-30</v>
       </c>
       <c r="P59" s="2">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>-29</v>
       </c>
       <c r="Q59" s="6">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>-28</v>
       </c>
       <c r="R59" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>-27</v>
       </c>
       <c r="S59" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>-26</v>
       </c>
       <c r="T59" s="6">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-25</v>
       </c>
       <c r="U59" s="6">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>-24</v>
       </c>
       <c r="V59" s="6">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-23</v>
       </c>
       <c r="W59" s="6">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>-22</v>
       </c>
       <c r="X59" s="6">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>-21</v>
       </c>
     </row>
@@ -3277,7 +3486,7 @@
         <v>43</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d3=43,</v>
       </c>
       <c r="K60" s="6">
@@ -3285,55 +3494,55 @@
         <v>-20</v>
       </c>
       <c r="L60" s="6">
-        <f t="shared" ref="L60:X60" si="65">L61-14</f>
+        <f t="shared" ref="L60:X60" si="66">L61-14</f>
         <v>-19</v>
       </c>
       <c r="M60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-18</v>
       </c>
       <c r="N60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-17</v>
       </c>
       <c r="O60" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-16</v>
       </c>
       <c r="P60" s="5">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-15</v>
       </c>
       <c r="Q60" s="4">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-14</v>
       </c>
       <c r="R60" s="5">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-13</v>
       </c>
       <c r="S60" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-12</v>
       </c>
       <c r="T60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-11</v>
       </c>
       <c r="U60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-10</v>
       </c>
       <c r="V60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-9</v>
       </c>
       <c r="W60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-8</v>
       </c>
       <c r="X60" s="6">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>-7</v>
       </c>
     </row>
@@ -3345,7 +3554,7 @@
         <v>44</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e3=44,</v>
       </c>
       <c r="K61" s="6">
@@ -3399,7 +3608,7 @@
         <v>45</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f3=45,</v>
       </c>
       <c r="K62" s="6">
@@ -3407,55 +3616,55 @@
         <v>8</v>
       </c>
       <c r="L62" s="6">
-        <f t="shared" ref="L62:X62" si="66">L61+14</f>
+        <f t="shared" ref="L62:X62" si="67">L61+14</f>
         <v>9</v>
       </c>
       <c r="M62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="N62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>11</v>
       </c>
       <c r="O62" s="2">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>12</v>
       </c>
       <c r="P62" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>13</v>
       </c>
       <c r="Q62" s="4">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>14</v>
       </c>
       <c r="R62" s="5">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="S62" s="2">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>16</v>
       </c>
       <c r="T62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>17</v>
       </c>
       <c r="U62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>18</v>
       </c>
       <c r="V62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>19</v>
       </c>
       <c r="W62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>20</v>
       </c>
       <c r="X62" s="6">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>21</v>
       </c>
     </row>
@@ -3467,63 +3676,63 @@
         <v>46</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g3=46,</v>
       </c>
       <c r="K63" s="6">
-        <f t="shared" ref="K63:K69" si="67">K62+14</f>
+        <f t="shared" ref="K63:K69" si="68">K62+14</f>
         <v>22</v>
       </c>
       <c r="L63" s="6">
-        <f t="shared" ref="L63:L69" si="68">L62+14</f>
+        <f t="shared" ref="L63:L69" si="69">L62+14</f>
         <v>23</v>
       </c>
       <c r="M63" s="6">
-        <f t="shared" ref="M63:M69" si="69">M62+14</f>
+        <f t="shared" ref="M63:M69" si="70">M62+14</f>
         <v>24</v>
       </c>
       <c r="N63" s="6">
-        <f t="shared" ref="N63:N69" si="70">N62+14</f>
+        <f t="shared" ref="N63:N69" si="71">N62+14</f>
         <v>25</v>
       </c>
       <c r="O63" s="6">
-        <f t="shared" ref="O63:O69" si="71">O62+14</f>
+        <f t="shared" ref="O63:O69" si="72">O62+14</f>
         <v>26</v>
       </c>
       <c r="P63" s="2">
-        <f t="shared" ref="P63:P69" si="72">P62+14</f>
+        <f t="shared" ref="P63:P69" si="73">P62+14</f>
         <v>27</v>
       </c>
       <c r="Q63" s="6">
-        <f t="shared" ref="Q63:Q69" si="73">Q62+14</f>
+        <f t="shared" ref="Q63:Q69" si="74">Q62+14</f>
         <v>28</v>
       </c>
       <c r="R63" s="2">
-        <f t="shared" ref="R63:R69" si="74">R62+14</f>
+        <f t="shared" ref="R63:R69" si="75">R62+14</f>
         <v>29</v>
       </c>
       <c r="S63" s="6">
-        <f t="shared" ref="S63:S69" si="75">S62+14</f>
+        <f t="shared" ref="S63:S69" si="76">S62+14</f>
         <v>30</v>
       </c>
       <c r="T63" s="6">
-        <f t="shared" ref="T63:T69" si="76">T62+14</f>
+        <f t="shared" ref="T63:T69" si="77">T62+14</f>
         <v>31</v>
       </c>
       <c r="U63" s="6">
-        <f t="shared" ref="U63:U69" si="77">U62+14</f>
+        <f t="shared" ref="U63:U69" si="78">U62+14</f>
         <v>32</v>
       </c>
       <c r="V63" s="6">
-        <f t="shared" ref="V63:V69" si="78">V62+14</f>
+        <f t="shared" ref="V63:V69" si="79">V62+14</f>
         <v>33</v>
       </c>
       <c r="W63" s="6">
-        <f t="shared" ref="W63:W69" si="79">W62+14</f>
+        <f t="shared" ref="W63:W69" si="80">W62+14</f>
         <v>34</v>
       </c>
       <c r="X63" s="6">
-        <f t="shared" ref="X63:X69" si="80">X62+14</f>
+        <f t="shared" ref="X63:X69" si="81">X62+14</f>
         <v>35</v>
       </c>
     </row>
@@ -3535,63 +3744,63 @@
         <v>47</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h3=47,</v>
       </c>
       <c r="K64" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>36</v>
       </c>
       <c r="L64" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>37</v>
       </c>
       <c r="M64" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>38</v>
       </c>
       <c r="N64" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>39</v>
       </c>
       <c r="O64" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>40</v>
       </c>
       <c r="P64" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>41</v>
       </c>
       <c r="Q64" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>42</v>
       </c>
       <c r="R64" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>43</v>
       </c>
       <c r="S64" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>44</v>
       </c>
       <c r="T64" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>45</v>
       </c>
       <c r="U64" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>46</v>
       </c>
       <c r="V64" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>47</v>
       </c>
       <c r="W64" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>48</v>
       </c>
       <c r="X64" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>49</v>
       </c>
     </row>
@@ -3603,63 +3812,63 @@
         <v>48</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a2=48,</v>
       </c>
       <c r="K65" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>50</v>
       </c>
       <c r="L65" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>51</v>
       </c>
       <c r="M65" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>52</v>
       </c>
       <c r="N65" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>53</v>
       </c>
       <c r="O65" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>54</v>
       </c>
       <c r="P65" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>55</v>
       </c>
       <c r="Q65" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>56</v>
       </c>
       <c r="R65" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>57</v>
       </c>
       <c r="S65" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>58</v>
       </c>
       <c r="T65" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>59</v>
       </c>
       <c r="U65" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>60</v>
       </c>
       <c r="V65" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>61</v>
       </c>
       <c r="W65" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>62</v>
       </c>
       <c r="X65" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>63</v>
       </c>
     </row>
@@ -3671,63 +3880,63 @@
         <v>49</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b2=49,</v>
       </c>
       <c r="K66" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>64</v>
       </c>
       <c r="L66" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>65</v>
       </c>
       <c r="M66" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>66</v>
       </c>
       <c r="N66" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>67</v>
       </c>
       <c r="O66" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>68</v>
       </c>
       <c r="P66" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>69</v>
       </c>
       <c r="Q66" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>70</v>
       </c>
       <c r="R66" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>71</v>
       </c>
       <c r="S66" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>72</v>
       </c>
       <c r="T66" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>73</v>
       </c>
       <c r="U66" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>74</v>
       </c>
       <c r="V66" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>75</v>
       </c>
       <c r="W66" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>76</v>
       </c>
       <c r="X66" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>77</v>
       </c>
     </row>
@@ -3739,63 +3948,63 @@
         <v>50</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c2=50,</v>
       </c>
       <c r="K67" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>78</v>
       </c>
       <c r="L67" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>79</v>
       </c>
       <c r="M67" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>80</v>
       </c>
       <c r="N67" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>81</v>
       </c>
       <c r="O67" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>82</v>
       </c>
       <c r="P67" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>83</v>
       </c>
       <c r="Q67" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>84</v>
       </c>
       <c r="R67" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>85</v>
       </c>
       <c r="S67" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>86</v>
       </c>
       <c r="T67" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>87</v>
       </c>
       <c r="U67" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>88</v>
       </c>
       <c r="V67" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>89</v>
       </c>
       <c r="W67" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>90</v>
       </c>
       <c r="X67" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>91</v>
       </c>
     </row>
@@ -3807,63 +4016,63 @@
         <v>51</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d2=51,</v>
       </c>
       <c r="K68" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>92</v>
       </c>
       <c r="L68" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>93</v>
       </c>
       <c r="M68" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>94</v>
       </c>
       <c r="N68" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>95</v>
       </c>
       <c r="O68" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>96</v>
       </c>
       <c r="P68" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>97</v>
       </c>
       <c r="Q68" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>98</v>
       </c>
       <c r="R68" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>99</v>
       </c>
       <c r="S68" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>100</v>
       </c>
       <c r="T68" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>101</v>
       </c>
       <c r="U68" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>102</v>
       </c>
       <c r="V68" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>103</v>
       </c>
       <c r="W68" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>104</v>
       </c>
       <c r="X68" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>105</v>
       </c>
     </row>
@@ -3875,63 +4084,63 @@
         <v>52</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e2=52,</v>
       </c>
       <c r="K69" s="6">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>106</v>
       </c>
       <c r="L69" s="6">
-        <f t="shared" si="68"/>
+        <f t="shared" si="69"/>
         <v>107</v>
       </c>
       <c r="M69" s="6">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>108</v>
       </c>
       <c r="N69" s="6">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>109</v>
       </c>
       <c r="O69" s="6">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>110</v>
       </c>
       <c r="P69" s="6">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>111</v>
       </c>
       <c r="Q69" s="6">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>112</v>
       </c>
       <c r="R69" s="6">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>113</v>
       </c>
       <c r="S69" s="6">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>114</v>
       </c>
       <c r="T69" s="6">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>115</v>
       </c>
       <c r="U69" s="6">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>116</v>
       </c>
       <c r="V69" s="6">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>117</v>
       </c>
       <c r="W69" s="6">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>118</v>
       </c>
       <c r="X69" s="6">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>119</v>
       </c>
     </row>
@@ -3943,7 +4152,7 @@
         <v>53</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f2=53,</v>
       </c>
     </row>
@@ -3955,7 +4164,7 @@
         <v>54</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g2=54,</v>
       </c>
       <c r="N71" s="6">
@@ -3963,31 +4172,31 @@
         <v>45</v>
       </c>
       <c r="O71" s="6">
-        <f t="shared" ref="O71:U71" si="81">O44+45+(6*_xlfn.FLOOR.MATH(O44/8))</f>
+        <f t="shared" ref="O71:U71" si="82">O44+45+(6*_xlfn.FLOOR.MATH(O44/8))</f>
         <v>46</v>
       </c>
       <c r="P71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>47</v>
       </c>
       <c r="Q71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>48</v>
       </c>
       <c r="R71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>49</v>
       </c>
       <c r="S71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>50</v>
       </c>
       <c r="T71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>51</v>
       </c>
       <c r="U71" s="6">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>52</v>
       </c>
       <c r="V71" s="6"/>
@@ -4001,39 +4210,39 @@
         <v>55</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h2=55,</v>
       </c>
       <c r="N72" s="6">
-        <f t="shared" ref="N72:U72" si="82">N45+45+(6*_xlfn.FLOOR.MATH(N45/8))</f>
+        <f t="shared" ref="N72:U72" si="83">N45+45+(6*_xlfn.FLOOR.MATH(N45/8))</f>
         <v>59</v>
       </c>
       <c r="O72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>60</v>
       </c>
       <c r="P72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>61</v>
       </c>
       <c r="Q72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>62</v>
       </c>
       <c r="R72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>63</v>
       </c>
       <c r="S72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>64</v>
       </c>
       <c r="T72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>65</v>
       </c>
       <c r="U72" s="6">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>66</v>
       </c>
     </row>
@@ -4045,39 +4254,39 @@
         <v>56</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>a1=56,</v>
       </c>
       <c r="N73" s="6">
-        <f t="shared" ref="N73:U73" si="83">N46+45+(6*_xlfn.FLOOR.MATH(N46/8))</f>
+        <f t="shared" ref="N73:U73" si="84">N46+45+(6*_xlfn.FLOOR.MATH(N46/8))</f>
         <v>73</v>
       </c>
       <c r="O73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>74</v>
       </c>
       <c r="P73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>75</v>
       </c>
       <c r="Q73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>76</v>
       </c>
       <c r="R73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>77</v>
       </c>
       <c r="S73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>78</v>
       </c>
       <c r="T73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>79</v>
       </c>
       <c r="U73" s="6">
-        <f t="shared" si="83"/>
+        <f t="shared" si="84"/>
         <v>80</v>
       </c>
     </row>
@@ -4089,39 +4298,39 @@
         <v>57</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>b1=57,</v>
       </c>
       <c r="N74" s="6">
-        <f t="shared" ref="N74:U74" si="84">N47+45+(6*_xlfn.FLOOR.MATH(N47/8))</f>
+        <f t="shared" ref="N74:U74" si="85">N47+45+(6*_xlfn.FLOOR.MATH(N47/8))</f>
         <v>87</v>
       </c>
       <c r="O74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>88</v>
       </c>
       <c r="P74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>89</v>
       </c>
       <c r="Q74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>90</v>
       </c>
       <c r="R74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>91</v>
       </c>
       <c r="S74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>92</v>
       </c>
       <c r="T74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>93</v>
       </c>
       <c r="U74" s="6">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>94</v>
       </c>
     </row>
@@ -4133,39 +4342,39 @@
         <v>58</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>c1=58,</v>
       </c>
       <c r="N75" s="6">
-        <f t="shared" ref="N75:U75" si="85">N48+45+(6*_xlfn.FLOOR.MATH(N48/8))</f>
+        <f t="shared" ref="N75:U75" si="86">N48+45+(6*_xlfn.FLOOR.MATH(N48/8))</f>
         <v>101</v>
       </c>
       <c r="O75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>102</v>
       </c>
       <c r="P75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>103</v>
       </c>
       <c r="Q75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>104</v>
       </c>
       <c r="R75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>105</v>
       </c>
       <c r="S75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>106</v>
       </c>
       <c r="T75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>107</v>
       </c>
       <c r="U75" s="6">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>108</v>
       </c>
     </row>
@@ -4177,39 +4386,39 @@
         <v>59</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>d1=59,</v>
       </c>
       <c r="N76" s="6">
-        <f t="shared" ref="N76:U76" si="86">N49+45+(6*_xlfn.FLOOR.MATH(N49/8))</f>
+        <f t="shared" ref="N76:U76" si="87">N49+45+(6*_xlfn.FLOOR.MATH(N49/8))</f>
         <v>115</v>
       </c>
       <c r="O76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>116</v>
       </c>
       <c r="P76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>117</v>
       </c>
       <c r="Q76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>118</v>
       </c>
       <c r="R76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>119</v>
       </c>
       <c r="S76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>120</v>
       </c>
       <c r="T76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>121</v>
       </c>
       <c r="U76" s="6">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>122</v>
       </c>
     </row>
@@ -4221,39 +4430,39 @@
         <v>60</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>e1=60,</v>
       </c>
       <c r="N77" s="6">
-        <f t="shared" ref="N77:U77" si="87">N50+45+(6*_xlfn.FLOOR.MATH(N50/8))</f>
+        <f t="shared" ref="N77:U77" si="88">N50+45+(6*_xlfn.FLOOR.MATH(N50/8))</f>
         <v>129</v>
       </c>
       <c r="O77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>130</v>
       </c>
       <c r="P77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>131</v>
       </c>
       <c r="Q77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>132</v>
       </c>
       <c r="R77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>133</v>
       </c>
       <c r="S77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>134</v>
       </c>
       <c r="T77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>135</v>
       </c>
       <c r="U77" s="6">
-        <f t="shared" si="87"/>
+        <f t="shared" si="88"/>
         <v>136</v>
       </c>
     </row>
@@ -4265,39 +4474,39 @@
         <v>61</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>f1=61,</v>
       </c>
       <c r="N78" s="6">
-        <f t="shared" ref="N78:U78" si="88">N51+45+(6*_xlfn.FLOOR.MATH(N51/8))</f>
+        <f t="shared" ref="N78:U78" si="89">N51+45+(6*_xlfn.FLOOR.MATH(N51/8))</f>
         <v>143</v>
       </c>
       <c r="O78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>144</v>
       </c>
       <c r="P78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>145</v>
       </c>
       <c r="Q78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>146</v>
       </c>
       <c r="R78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>147</v>
       </c>
       <c r="S78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>148</v>
       </c>
       <c r="T78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>149</v>
       </c>
       <c r="U78" s="6">
-        <f t="shared" si="88"/>
+        <f t="shared" si="89"/>
         <v>150</v>
       </c>
     </row>
@@ -4309,7 +4518,7 @@
         <v>62</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>g1=62,</v>
       </c>
     </row>
@@ -4321,7 +4530,7 @@
         <v>63</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>h1=63,</v>
       </c>
       <c r="N80">
@@ -4539,115 +4748,380 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3890B13-C358-456C-98AE-7F6A57C46179}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B46">
+    <sortCondition ref="B2:B46"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>